<commit_message>
dataframe order by values, rename strategies, and others
</commit_message>
<xml_diff>
--- a/experiments/experiment_3/notebooks/estrategia1.xlsx
+++ b/experiments/experiment_3/notebooks/estrategia1.xlsx
@@ -85,28 +85,28 @@
     <t>final_accumulated_fmeasure</t>
   </si>
   <si>
+    <t>wiley</t>
+  </si>
+  <si>
+    <t>webofscience</t>
+  </si>
+  <si>
+    <t>springer</t>
+  </si>
+  <si>
+    <t>scopus</t>
+  </si>
+  <si>
+    <t>sciencedirect</t>
+  </si>
+  <si>
     <t>ieee</t>
   </si>
   <si>
-    <t>webofscience</t>
-  </si>
-  <si>
-    <t>wiley</t>
-  </si>
-  <si>
-    <t>sciencedirect</t>
+    <t>googlescholar</t>
   </si>
   <si>
     <t>acm</t>
-  </si>
-  <si>
-    <t>springer</t>
-  </si>
-  <si>
-    <t>scopus</t>
-  </si>
-  <si>
-    <t>googlescholar</t>
   </si>
   <si>
     <t>s0</t>
@@ -557,10 +557,16 @@
       <c r="B2" t="s">
         <v>23</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
@@ -576,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -585,13 +591,13 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -668,7 +674,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1.54</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -677,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>0.01538461538461539</v>
       </c>
       <c r="W3">
         <v>0</v>
@@ -694,13 +700,13 @@
         <v>25</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1.54</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>7.140000000000001</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>2.53</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -715,49 +721,49 @@
         <v>32</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1.54</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>7.140000000000001</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>2.53</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>0.01538461538461539</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>0.02531645569620253</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -768,13 +774,13 @@
         <v>26</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>21.43</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>6.45</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -789,49 +795,49 @@
         <v>32</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K5">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N5">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P5">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>21.43</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>6.45</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>0.0379746835443038</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <v>0.06451612903225806</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -841,10 +847,16 @@
       <c r="B6" t="s">
         <v>27</v>
       </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
@@ -860,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -869,13 +881,13 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -884,7 +896,7 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -893,7 +905,7 @@
         <v>0</v>
       </c>
       <c r="V6">
-        <v>0.01538461538461539</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -909,16 +921,10 @@
       <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C7">
-        <v>1.5</v>
-      </c>
       <c r="D7">
-        <v>7.1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>2.5</v>
-      </c>
-      <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
@@ -931,49 +937,49 @@
         <v>32</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <v>0</v>
       </c>
       <c r="S7">
-        <v>1.5</v>
+        <v>2.36</v>
       </c>
       <c r="T7">
-        <v>7.1</v>
+        <v>0</v>
       </c>
       <c r="U7">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="V7">
-        <v>0.01538461538461539</v>
+        <v>0.02360515021459228</v>
       </c>
       <c r="W7">
-        <v>0.07142857142857142</v>
+        <v>0</v>
       </c>
       <c r="X7">
-        <v>0.02531645569620253</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -984,13 +990,13 @@
         <v>29</v>
       </c>
       <c r="C8">
-        <v>3.8</v>
+        <v>2.36</v>
       </c>
       <c r="D8">
-        <v>21.4</v>
+        <v>78.56999999999999</v>
       </c>
       <c r="E8">
-        <v>6.5</v>
+        <v>4.58</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1005,49 +1011,49 @@
         <v>32</v>
       </c>
       <c r="J8">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="K8">
-        <v>79</v>
+        <v>466</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="N8">
-        <v>79</v>
+        <v>466</v>
       </c>
       <c r="O8">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="P8">
-        <v>2</v>
+        <v>466</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="R8">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>3.8</v>
+        <v>2.36</v>
       </c>
       <c r="T8">
-        <v>21.4</v>
+        <v>78.56999999999999</v>
       </c>
       <c r="U8">
-        <v>6.5</v>
+        <v>4.58</v>
       </c>
       <c r="V8">
-        <v>0.0379746835443038</v>
+        <v>0.02360515021459228</v>
       </c>
       <c r="W8">
-        <v>0.2142857142857143</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="X8">
-        <v>0.06451612903225806</v>
+        <v>0.04583333333333334</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -1057,16 +1063,10 @@
       <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9">
-        <v>2.4</v>
-      </c>
       <c r="D9">
-        <v>78.60000000000001</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>4.6</v>
-      </c>
-      <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
@@ -1079,49 +1079,49 @@
         <v>32</v>
       </c>
       <c r="J9">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>466</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>466</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>466</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="R9">
         <v>0</v>
       </c>
       <c r="S9">
-        <v>2.4</v>
+        <v>2.29</v>
       </c>
       <c r="T9">
-        <v>78.60000000000001</v>
+        <v>0</v>
       </c>
       <c r="U9">
-        <v>4.6</v>
+        <v>0</v>
       </c>
       <c r="V9">
-        <v>0.02360515021459228</v>
+        <v>0.02291666666666667</v>
       </c>
       <c r="W9">
-        <v>0.7857142857142857</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <v>0.04583333333333334</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -1174,13 +1174,13 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>2.3</v>
+        <v>2.29</v>
       </c>
       <c r="T10">
-        <v>78.60000000000001</v>
+        <v>78.56999999999999</v>
       </c>
       <c r="U10">
-        <v>4.5</v>
+        <v>4.45</v>
       </c>
       <c r="V10">
         <v>0.02291666666666667</v>

</xml_diff>